<commit_message>
Revise flow characteristics spreadsheet
- Specify actual measured pressure drop across orifice+3-way valve as
  pressure drop across MFC (this is a realistic, not minimum value)
- Increase resolution of calculated values table
- Change barometric pressure sea level -> Pullman (1976 std. atmos.)
</commit_message>
<xml_diff>
--- a/engr/flow_characteristics.xlsx
+++ b/engr/flow_characteristics.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="487"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Flow" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
@@ -22,6 +22,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
+    <author>Patrick O'Keeffe</author>
   </authors>
   <commentList>
     <comment ref="G1" authorId="0" shapeId="0">
@@ -156,6 +157,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Measured pressure drop across orifice+3-way valve as 19 in Hg = 9.3 psi</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
@@ -229,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -252,6 +277,32 @@
             <charset val="1"/>
           </rPr>
           <t>Max ratio of abs. press. downstream of orifice vs. abs. press. upstream of orifice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A34" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Patrick O'Keeffe:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Max absolute pressure downstream of orifice resulting in choked flow</t>
         </r>
       </text>
     </comment>
@@ -277,7 +328,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Max absolute pressure downstream of orifice resulting in choked flow</t>
+          <t>Minimum pressure drop across orifice to achieve choked flow</t>
         </r>
       </text>
     </comment>
@@ -303,37 +354,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Minimum pressure drop across orifice to achieve choked flow</t>
+          <t>Vacuum level resulting from pressure drop across mass flow controller and wall friction</t>
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Patrick O'Keeffe:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Vacuum level resulting from pressure drop across mass flow controller and wall friction</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B37" authorId="0" shapeId="0">
+    <comment ref="B36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -553,7 +578,7 @@
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -585,6 +610,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -600,7 +638,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -638,30 +676,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -692,7 +712,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -701,6 +720,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1543,10 +1565,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,64 +1577,64 @@
     <col min="2" max="2" width="12"/>
     <col min="3" max="3" width="14.28515625"/>
     <col min="4" max="4" width="2.140625"/>
-    <col min="5" max="5" width="5.85546875" style="2"/>
-    <col min="6" max="6" width="7.5703125" style="2"/>
-    <col min="7" max="7" width="6" style="2"/>
-    <col min="8" max="9" width="7.7109375" style="2"/>
-    <col min="10" max="10" width="10.5703125" style="2"/>
-    <col min="11" max="11" width="13.42578125" style="2"/>
-    <col min="12" max="12" width="9.5703125" style="2"/>
-    <col min="13" max="13" width="8.5703125" style="2"/>
+    <col min="5" max="5" width="5.85546875" style="1"/>
+    <col min="6" max="6" width="7.5703125" style="1"/>
+    <col min="7" max="7" width="6" style="1"/>
+    <col min="8" max="9" width="7.7109375" style="1"/>
+    <col min="10" max="10" width="10.5703125" style="1"/>
+    <col min="11" max="11" width="13.42578125" style="1"/>
+    <col min="12" max="12" width="9.5703125" style="1"/>
+    <col min="13" max="13" width="8.5703125" style="1"/>
     <col min="14" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="21"/>
       <c r="J1"/>
-      <c r="K1"/>
+      <c r="K1" s="2"/>
       <c r="L1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1621,45 +1643,45 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6">
-        <f t="shared" ref="F3:F21" si="0">E3*$B$23^2/($B$34*$B$24*$B$25)</f>
-        <v>34.226801028389069</v>
-      </c>
-      <c r="G3" s="7">
-        <f t="shared" ref="G3:G21" si="1">$B$11/(F3*$B$27)</f>
-        <v>0.17809734905288202</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H21" si="2">G3*1000/100</f>
-        <v>1.7809734905288201</v>
-      </c>
-      <c r="I3" s="8">
-        <f t="shared" ref="I3:I21" si="3">G3*1000/50</f>
-        <v>3.5619469810576403</v>
-      </c>
-      <c r="J3" s="6">
-        <f t="shared" ref="J3:J21" si="4">$B$32*F3*$B$10/($B$33*$B$23)</f>
-        <v>1828.6200539692495</v>
-      </c>
-      <c r="K3" s="9">
-        <f t="shared" ref="K3:K21" si="5">0.316/J3^0.25</f>
-        <v>4.8323258657599504E-2</v>
-      </c>
-      <c r="L3" s="7">
-        <f t="shared" ref="L3:L21" si="6">K3*$B$11*$B$32*$B$26*$B$21/(2*$B$10*$B$28)</f>
-        <v>2.2998972798131674</v>
-      </c>
-      <c r="M3" s="7">
+      <c r="E3" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" ref="F3:F21" si="0">E3*$B$22^2/($B$33*$B$23*$B$24)</f>
+        <v>58.185561748261414</v>
+      </c>
+      <c r="G3" s="6">
+        <f>$B$11/(F3*$B$26)</f>
+        <v>0.10476314650169533</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H21" si="1">G3*1000/100</f>
+        <v>1.0476314650169534</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I21" si="2">G3*1000/50</f>
+        <v>2.0952629300339067</v>
+      </c>
+      <c r="J3" s="5">
+        <f>$B$31*F3*$B$10/($B$32*$B$22)</f>
+        <v>2821.3251983118475</v>
+      </c>
+      <c r="K3" s="8">
+        <f t="shared" ref="K3:K21" si="3">0.316/J3^0.25</f>
+        <v>4.3358454718245489E-2</v>
+      </c>
+      <c r="L3" s="6">
+        <f>K3*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.8728662793168234</v>
+      </c>
+      <c r="M3" s="6">
         <f>100*(2*6/1000)/E3</f>
-        <v>1.2</v>
+        <v>0.70588235294117652</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1669,44 +1691,44 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5">
-        <v>2</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="F4" s="5">
         <f t="shared" si="0"/>
-        <v>68.453602056778138</v>
-      </c>
-      <c r="G4" s="7">
+        <v>61.608241851100324</v>
+      </c>
+      <c r="G4" s="6">
+        <f>$B$11/(F4*$B$26)</f>
+        <v>9.8942971696045573E-2</v>
+      </c>
+      <c r="H4" s="7">
         <f t="shared" si="1"/>
-        <v>8.904867452644101E-2</v>
-      </c>
-      <c r="H4" s="8">
+        <v>0.98942971696045579</v>
+      </c>
+      <c r="I4" s="7">
         <f t="shared" si="2"/>
-        <v>0.89048674526441007</v>
-      </c>
-      <c r="I4" s="8">
+        <v>1.9788594339209116</v>
+      </c>
+      <c r="J4" s="5">
+        <f>$B$31*F4*$B$10/($B$32*$B$22)</f>
+        <v>2987.2855040948975</v>
+      </c>
+      <c r="K4" s="8">
         <f t="shared" si="3"/>
-        <v>1.7809734905288201</v>
-      </c>
-      <c r="J4" s="6">
-        <f t="shared" si="4"/>
-        <v>3657.240107938499</v>
-      </c>
-      <c r="K4" s="9">
-        <f t="shared" si="5"/>
-        <v>4.0634854978553445E-2</v>
-      </c>
-      <c r="L4" s="7">
-        <f t="shared" si="6"/>
-        <v>1.9339753780466613</v>
-      </c>
-      <c r="M4" s="7">
-        <f t="shared" ref="M4:M21" si="7">100*(2*6/1000)/E4</f>
-        <v>0.6</v>
+        <v>4.2743285324756887E-2</v>
+      </c>
+      <c r="L4" s="6">
+        <f>K4*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.8462940681847746</v>
+      </c>
+      <c r="M4" s="6">
+        <f t="shared" ref="M4:M21" si="4">100*(2*6/1000)/E4</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B5">
@@ -1716,44 +1738,44 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5">
-        <v>3</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="E5" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>102.6804030851672</v>
-      </c>
-      <c r="G5" s="7">
+        <v>65.030921953939227</v>
+      </c>
+      <c r="G5" s="6">
+        <f>$B$11/(F5*$B$26)</f>
+        <v>9.3735446869937913E-2</v>
+      </c>
+      <c r="H5" s="7">
         <f t="shared" si="1"/>
-        <v>5.9365783017627342E-2</v>
-      </c>
-      <c r="H5" s="8">
+        <v>0.93735446869937922</v>
+      </c>
+      <c r="I5" s="7">
         <f t="shared" si="2"/>
-        <v>0.59365783017627338</v>
-      </c>
-      <c r="I5" s="8">
+        <v>1.8747089373987584</v>
+      </c>
+      <c r="J5" s="5">
+        <f>$B$31*F5*$B$10/($B$32*$B$22)</f>
+        <v>3153.2458098779475</v>
+      </c>
+      <c r="K5" s="8">
         <f t="shared" si="3"/>
-        <v>1.1873156603525468</v>
-      </c>
-      <c r="J5" s="6">
+        <v>4.2169419809878761E-2</v>
+      </c>
+      <c r="L5" s="6">
+        <f>K5*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.8215059760200014</v>
+      </c>
+      <c r="M5" s="6">
         <f t="shared" si="4"/>
-        <v>5485.860161907749</v>
-      </c>
-      <c r="K5" s="9">
-        <f t="shared" si="5"/>
-        <v>3.6717736375016373E-2</v>
-      </c>
-      <c r="L5" s="7">
-        <f t="shared" si="6"/>
-        <v>1.7475440265350708</v>
-      </c>
-      <c r="M5" s="7">
-        <f t="shared" si="7"/>
-        <v>0.39999999999999997</v>
+        <v>0.63157894736842102</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B6">
@@ -1763,44 +1785,44 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="5">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>136.90720411355628</v>
-      </c>
-      <c r="G6" s="7">
+        <v>68.453602056778138</v>
+      </c>
+      <c r="G6" s="6">
+        <f>$B$11/(F6*$B$26)</f>
+        <v>8.904867452644101E-2</v>
+      </c>
+      <c r="H6" s="7">
         <f t="shared" si="1"/>
-        <v>4.4524337263220505E-2</v>
-      </c>
-      <c r="H6" s="8">
+        <v>0.89048674526441007</v>
+      </c>
+      <c r="I6" s="7">
         <f t="shared" si="2"/>
-        <v>0.44524337263220504</v>
-      </c>
-      <c r="I6" s="8">
+        <v>1.7809734905288201</v>
+      </c>
+      <c r="J6" s="5">
+        <f>$B$31*F6*$B$10/($B$32*$B$22)</f>
+        <v>3319.206115660998</v>
+      </c>
+      <c r="K6" s="8">
         <f t="shared" si="3"/>
-        <v>0.89048674526441007</v>
-      </c>
-      <c r="J6" s="6">
+        <v>4.1632120040838612E-2</v>
+      </c>
+      <c r="L6" s="6">
+        <f>K6*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.798297339414773</v>
+      </c>
+      <c r="M6" s="6">
         <f t="shared" si="4"/>
-        <v>7314.480215876998</v>
-      </c>
-      <c r="K6" s="9">
-        <f t="shared" si="5"/>
-        <v>3.4169703885820149E-2</v>
-      </c>
-      <c r="L6" s="7">
-        <f t="shared" si="6"/>
-        <v>1.6262729625883849</v>
-      </c>
-      <c r="M6" s="7">
-        <f t="shared" si="7"/>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B7">
@@ -1810,810 +1832,807 @@
       <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="5">
-        <v>5</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="E7" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>171.13400514194535</v>
-      </c>
-      <c r="G7" s="7">
+        <v>71.876282159617048</v>
+      </c>
+      <c r="G7" s="6">
+        <f>$B$11/(F7*$B$26)</f>
+        <v>8.4808261453753336E-2</v>
+      </c>
+      <c r="H7" s="7">
         <f t="shared" si="1"/>
-        <v>3.5619469810576405E-2</v>
-      </c>
-      <c r="H7" s="8">
+        <v>0.84808261453753331</v>
+      </c>
+      <c r="I7" s="7">
         <f t="shared" si="2"/>
-        <v>0.35619469810576404</v>
-      </c>
-      <c r="I7" s="8">
+        <v>1.6961652290750666</v>
+      </c>
+      <c r="J7" s="5">
+        <f>$B$31*F7*$B$10/($B$32*$B$22)</f>
+        <v>3485.1664214440475</v>
+      </c>
+      <c r="K7" s="8">
         <f t="shared" si="3"/>
-        <v>0.71238939621152808</v>
-      </c>
-      <c r="J7" s="6">
+        <v>4.1127395007846616E-2</v>
+      </c>
+      <c r="L7" s="6">
+        <f>K7*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.7764957669011656</v>
+      </c>
+      <c r="M7" s="6">
         <f t="shared" si="4"/>
-        <v>9143.1002698462471</v>
-      </c>
-      <c r="K7" s="9">
-        <f t="shared" si="5"/>
-        <v>3.2315710732137626E-2</v>
-      </c>
-      <c r="L7" s="7">
-        <f t="shared" si="6"/>
-        <v>1.538034008316701</v>
-      </c>
-      <c r="M7" s="7">
-        <f t="shared" si="7"/>
-        <v>0.24</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E8" s="5">
-        <v>6</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="E8" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>205.3608061703344</v>
-      </c>
-      <c r="G8" s="7">
+        <v>75.298962262455959</v>
+      </c>
+      <c r="G8" s="6">
+        <f>$B$11/(F8*$B$26)</f>
+        <v>8.0953340478582742E-2</v>
+      </c>
+      <c r="H8" s="7">
         <f t="shared" si="1"/>
-        <v>2.9682891508813671E-2</v>
-      </c>
-      <c r="H8" s="8">
+        <v>0.80953340478582747</v>
+      </c>
+      <c r="I8" s="7">
         <f t="shared" si="2"/>
-        <v>0.29682891508813669</v>
-      </c>
-      <c r="I8" s="8">
+        <v>1.6190668095716549</v>
+      </c>
+      <c r="J8" s="5">
+        <f>$B$31*F8*$B$10/($B$32*$B$22)</f>
+        <v>3651.126727227097</v>
+      </c>
+      <c r="K8" s="8">
         <f t="shared" si="3"/>
-        <v>0.59365783017627338</v>
-      </c>
-      <c r="J8" s="6">
+        <v>4.0651853875771964E-2</v>
+      </c>
+      <c r="L8" s="6">
+        <f>K8*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.7559547915255838</v>
+      </c>
+      <c r="M8" s="6">
         <f t="shared" si="4"/>
-        <v>10971.720323815498</v>
-      </c>
-      <c r="K8" s="9">
-        <f t="shared" si="5"/>
-        <v>3.0875812893982189E-2</v>
-      </c>
-      <c r="L8" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4695035074113831</v>
-      </c>
-      <c r="M8" s="7">
-        <f t="shared" si="7"/>
-        <v>0.19999999999999998</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="5">
-        <v>7</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="E9" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
-        <v>239.58760719872348</v>
-      </c>
-      <c r="G9" s="7">
+        <v>78.721642365294855</v>
+      </c>
+      <c r="G9" s="6">
+        <f>$B$11/(F9*$B$26)</f>
+        <v>7.7433630022992195E-2</v>
+      </c>
+      <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>2.5442478436126004E-2</v>
-      </c>
-      <c r="H9" s="8">
+        <v>0.77433630022992195</v>
+      </c>
+      <c r="I9" s="7">
         <f t="shared" si="2"/>
-        <v>0.25442478436126004</v>
-      </c>
-      <c r="I9" s="8">
+        <v>1.5486726004598439</v>
+      </c>
+      <c r="J9" s="5">
+        <f>$B$31*F9*$B$10/($B$32*$B$22)</f>
+        <v>3817.0870330101475</v>
+      </c>
+      <c r="K9" s="8">
         <f t="shared" si="3"/>
-        <v>0.50884956872252007</v>
-      </c>
-      <c r="J9" s="6">
+        <v>4.0202593163982538E-2</v>
+      </c>
+      <c r="L9" s="6">
+        <f>K9*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.7365489975875856</v>
+      </c>
+      <c r="M9" s="6">
         <f t="shared" si="4"/>
-        <v>12800.340377784749</v>
-      </c>
-      <c r="K9" s="9">
-        <f t="shared" si="5"/>
-        <v>2.9708566934691791E-2</v>
-      </c>
-      <c r="L9" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4139496006339745</v>
-      </c>
-      <c r="M9" s="7">
-        <f t="shared" si="7"/>
-        <v>0.17142857142857143</v>
+        <v>0.52173913043478259</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>3.1E-2</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="5">
-        <v>8</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="E10" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
-        <v>273.81440822711255</v>
-      </c>
-      <c r="G10" s="7">
+        <v>82.144322468133765</v>
+      </c>
+      <c r="G10" s="6">
+        <f>$B$11/(F10*$B$26)</f>
+        <v>7.4207228772034173E-2</v>
+      </c>
+      <c r="H10" s="7">
         <f t="shared" si="1"/>
-        <v>2.2262168631610253E-2</v>
-      </c>
-      <c r="H10" s="8">
+        <v>0.74207228772034173</v>
+      </c>
+      <c r="I10" s="7">
         <f t="shared" si="2"/>
-        <v>0.22262168631610252</v>
-      </c>
-      <c r="I10" s="8">
+        <v>1.4841445754406835</v>
+      </c>
+      <c r="J10" s="5">
+        <f>$B$31*F10*$B$10/($B$32*$B$22)</f>
+        <v>3983.047338793197</v>
+      </c>
+      <c r="K10" s="8">
         <f t="shared" si="3"/>
-        <v>0.44524337263220504</v>
-      </c>
-      <c r="J10" s="6">
+        <v>3.9777109017206221E-2</v>
+      </c>
+      <c r="L10" s="6">
+        <f>K10*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.7181702311841345</v>
+      </c>
+      <c r="M10" s="6">
         <f t="shared" si="4"/>
-        <v>14628.960431753996</v>
-      </c>
-      <c r="K10" s="9">
-        <f t="shared" si="5"/>
-        <v>2.8733181507867082E-2</v>
-      </c>
-      <c r="L10" s="7">
-        <f t="shared" si="6"/>
-        <v>1.3675271044646111</v>
-      </c>
-      <c r="M10" s="7">
-        <f t="shared" si="7"/>
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="5">
-        <v>9</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="E11" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>308.0412092555016</v>
-      </c>
-      <c r="G11" s="7">
+        <v>85.567002570972676</v>
+      </c>
+      <c r="G11" s="6">
+        <f>$B$11/(F11*$B$26)</f>
+        <v>7.1238939621152811E-2</v>
+      </c>
+      <c r="H11" s="7">
         <f t="shared" si="1"/>
-        <v>1.9788594339209115E-2</v>
-      </c>
-      <c r="H11" s="8">
+        <v>0.71238939621152808</v>
+      </c>
+      <c r="I11" s="7">
         <f t="shared" si="2"/>
-        <v>0.19788594339209115</v>
-      </c>
-      <c r="I11" s="8">
+        <v>1.4247787924230562</v>
+      </c>
+      <c r="J11" s="5">
+        <f>$B$31*F11*$B$10/($B$32*$B$22)</f>
+        <v>4149.007644576247</v>
+      </c>
+      <c r="K11" s="8">
         <f t="shared" si="3"/>
-        <v>0.39577188678418229</v>
-      </c>
-      <c r="J11" s="6">
+        <v>3.9373228193636083E-2</v>
+      </c>
+      <c r="L11" s="6">
+        <f>K11*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.700724619244258</v>
+      </c>
+      <c r="M11" s="6">
         <f t="shared" si="4"/>
-        <v>16457.580485723247</v>
-      </c>
-      <c r="K11" s="9">
-        <f t="shared" si="5"/>
-        <v>2.7899446394084992E-2</v>
-      </c>
-      <c r="L11" s="7">
-        <f t="shared" si="6"/>
-        <v>1.32784631360862</v>
-      </c>
-      <c r="M11" s="7">
-        <f t="shared" si="7"/>
-        <v>0.13333333333333333</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="13">
-        <v>101.7</v>
+      <c r="B12" s="12">
+        <v>92.3</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="5">
-        <v>10</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="E12" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>342.2680102838907</v>
-      </c>
-      <c r="G12" s="7">
+        <v>88.989682673811572</v>
+      </c>
+      <c r="G12" s="6">
+        <f>$B$11/(F12*$B$26)</f>
+        <v>6.849898040495464E-2</v>
+      </c>
+      <c r="H12" s="7">
         <f t="shared" si="1"/>
-        <v>1.7809734905288203E-2</v>
-      </c>
-      <c r="H12" s="8">
+        <v>0.68498980404954635</v>
+      </c>
+      <c r="I12" s="7">
         <f t="shared" si="2"/>
-        <v>0.17809734905288202</v>
-      </c>
-      <c r="I12" s="8">
+        <v>1.3699796080990927</v>
+      </c>
+      <c r="J12" s="5">
+        <f>$B$31*F12*$B$10/($B$32*$B$22)</f>
+        <v>4314.967950359297</v>
+      </c>
+      <c r="K12" s="8">
         <f t="shared" si="3"/>
-        <v>0.35619469810576404</v>
-      </c>
-      <c r="J12" s="6">
+        <v>3.8989053201482479E-2</v>
+      </c>
+      <c r="L12" s="6">
+        <f>K12*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.6841301997051659</v>
+      </c>
+      <c r="M12" s="6">
         <f t="shared" si="4"/>
-        <v>18286.200539692494</v>
-      </c>
-      <c r="K12" s="9">
-        <f t="shared" si="5"/>
-        <v>2.7174165311030517E-2</v>
-      </c>
-      <c r="L12" s="7">
-        <f t="shared" si="6"/>
-        <v>1.2933272841318155</v>
-      </c>
-      <c r="M12" s="7">
-        <f t="shared" si="7"/>
-        <v>0.12</v>
+        <v>0.46153846153846151</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="5">
-        <v>11</v>
-      </c>
-      <c r="F13" s="6">
+      <c r="E13" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>376.49481131227975</v>
-      </c>
-      <c r="G13" s="7">
+        <v>92.412362776650482</v>
+      </c>
+      <c r="G13" s="6">
+        <f>$B$11/(F13*$B$26)</f>
+        <v>6.5961981130697039E-2</v>
+      </c>
+      <c r="H13" s="7">
         <f t="shared" si="1"/>
-        <v>1.6190668095716548E-2</v>
-      </c>
-      <c r="H13" s="8">
+        <v>0.65961981130697045</v>
+      </c>
+      <c r="I13" s="7">
         <f t="shared" si="2"/>
-        <v>0.16190668095716546</v>
-      </c>
-      <c r="I13" s="8">
+        <v>1.3192396226139409</v>
+      </c>
+      <c r="J13" s="5">
+        <f>$B$31*F13*$B$10/($B$32*$B$22)</f>
+        <v>4480.9282561423461</v>
+      </c>
+      <c r="K13" s="8">
         <f t="shared" si="3"/>
-        <v>0.32381336191433091</v>
-      </c>
-      <c r="J13" s="6">
+        <v>3.8622918260317607E-2</v>
+      </c>
+      <c r="L13" s="6">
+        <f>K13*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.6683150192647342</v>
+      </c>
+      <c r="M13" s="6">
         <f t="shared" si="4"/>
-        <v>20114.820593661745</v>
-      </c>
-      <c r="K13" s="9">
-        <f t="shared" si="5"/>
-        <v>2.6534324851495875E-2</v>
-      </c>
-      <c r="L13" s="7">
-        <f t="shared" si="6"/>
-        <v>1.262874715880467</v>
-      </c>
-      <c r="M13" s="7">
-        <f t="shared" si="7"/>
-        <v>0.10909090909090909</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="E14" s="5">
-        <v>12</v>
-      </c>
-      <c r="F14" s="6">
+      <c r="E14" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>410.7216123406688</v>
-      </c>
-      <c r="G14" s="7">
+        <v>95.835042879489379</v>
+      </c>
+      <c r="G14" s="6">
+        <f>$B$11/(F14*$B$26)</f>
+        <v>6.3606196090315023E-2</v>
+      </c>
+      <c r="H14" s="7">
         <f t="shared" si="1"/>
-        <v>1.4841445754406836E-2</v>
-      </c>
-      <c r="H14" s="8">
+        <v>0.63606196090315026</v>
+      </c>
+      <c r="I14" s="7">
         <f t="shared" si="2"/>
-        <v>0.14841445754406835</v>
-      </c>
-      <c r="I14" s="8">
+        <v>1.2721239218063005</v>
+      </c>
+      <c r="J14" s="5">
+        <f>$B$31*F14*$B$10/($B$32*$B$22)</f>
+        <v>4646.8885619253961</v>
+      </c>
+      <c r="K14" s="8">
         <f t="shared" si="3"/>
-        <v>0.29682891508813669</v>
-      </c>
-      <c r="J14" s="6">
+        <v>3.8273353636513498E-2</v>
+      </c>
+      <c r="L14" s="6">
+        <f>K14*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.6532155928525358</v>
+      </c>
+      <c r="M14" s="6">
         <f t="shared" si="4"/>
-        <v>21943.440647630996</v>
-      </c>
-      <c r="K14" s="9">
-        <f t="shared" si="5"/>
-        <v>2.5963360380594044E-2</v>
-      </c>
-      <c r="L14" s="7">
-        <f t="shared" si="6"/>
-        <v>1.2357002315849923</v>
-      </c>
-      <c r="M14" s="7">
-        <f t="shared" si="7"/>
-        <v>9.9999999999999992E-2</v>
+        <v>0.4285714285714286</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E15" s="5">
-        <v>13</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="F15" s="5">
         <f t="shared" si="0"/>
-        <v>444.9484133690579</v>
-      </c>
-      <c r="G15" s="7">
+        <v>99.257722982328303</v>
+      </c>
+      <c r="G15" s="6">
+        <f>$B$11/(F15*$B$26)</f>
+        <v>6.1412878983752424E-2</v>
+      </c>
+      <c r="H15" s="7">
         <f t="shared" si="1"/>
-        <v>1.3699796080990924E-2</v>
-      </c>
-      <c r="H15" s="8">
+        <v>0.61412878983752417</v>
+      </c>
+      <c r="I15" s="7">
         <f t="shared" si="2"/>
-        <v>0.13699796080990922</v>
-      </c>
-      <c r="I15" s="8">
+        <v>1.2282575796750483</v>
+      </c>
+      <c r="J15" s="5">
+        <f>$B$31*F15*$B$10/($B$32*$B$22)</f>
+        <v>4812.848867708447</v>
+      </c>
+      <c r="K15" s="8">
         <f t="shared" si="3"/>
-        <v>0.27399592161981845</v>
-      </c>
-      <c r="J15" s="6">
+        <v>3.7939056523227585E-2</v>
+      </c>
+      <c r="L15" s="6">
+        <f>K15*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.638775645792276</v>
+      </c>
+      <c r="M15" s="6">
         <f t="shared" si="4"/>
-        <v>23772.060701600243</v>
-      </c>
-      <c r="K15" s="9">
-        <f t="shared" si="5"/>
-        <v>2.5448979681513884E-2</v>
-      </c>
-      <c r="L15" s="7">
-        <f t="shared" si="6"/>
-        <v>1.2112187954511979</v>
-      </c>
-      <c r="M15" s="7">
-        <f t="shared" si="7"/>
-        <v>9.2307692307692299E-2</v>
+        <v>0.41379310344827586</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="5">
-        <v>14</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="13">
+        <v>287.05799999999999</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3</v>
+      </c>
+      <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>479.17521439744695</v>
-      </c>
-      <c r="G16" s="7">
+        <v>102.6804030851672</v>
+      </c>
+      <c r="G16" s="6">
+        <f>$B$11/(F16*$B$26)</f>
+        <v>5.9365783017627342E-2</v>
+      </c>
+      <c r="H16" s="7">
         <f t="shared" si="1"/>
-        <v>1.2721239218063002E-2</v>
-      </c>
-      <c r="H16" s="8">
+        <v>0.59365783017627338</v>
+      </c>
+      <c r="I16" s="7">
         <f t="shared" si="2"/>
-        <v>0.12721239218063002</v>
-      </c>
-      <c r="I16" s="8">
+        <v>1.1873156603525468</v>
+      </c>
+      <c r="J16" s="5">
+        <f>$B$31*F16*$B$10/($B$32*$B$22)</f>
+        <v>4978.809173491496</v>
+      </c>
+      <c r="K16" s="8">
         <f t="shared" si="3"/>
-        <v>0.25442478436126004</v>
-      </c>
-      <c r="J16" s="6">
+        <v>3.7618867083427356E-2</v>
+      </c>
+      <c r="L16" s="6">
+        <f>K16*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.6249450789814421</v>
+      </c>
+      <c r="M16" s="6">
         <f t="shared" si="4"/>
-        <v>25600.680755569498</v>
-      </c>
-      <c r="K16" s="9">
-        <f t="shared" si="5"/>
-        <v>2.4981827437707362E-2</v>
-      </c>
-      <c r="L16" s="7">
-        <f t="shared" si="6"/>
-        <v>1.1889851505225304</v>
-      </c>
-      <c r="M16" s="7">
-        <f t="shared" si="7"/>
-        <v>8.5714285714285715E-2</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="15">
-        <v>287.05799999999999</v>
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="5">
-        <v>15</v>
-      </c>
-      <c r="F17" s="6">
+        <v>33</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>513.402015425836</v>
-      </c>
-      <c r="G17" s="7">
+        <v>106.10308318800611</v>
+      </c>
+      <c r="G17" s="6">
+        <f>$B$11/(F17*$B$26)</f>
+        <v>5.7450757758994206E-2</v>
+      </c>
+      <c r="H17" s="7">
         <f t="shared" si="1"/>
-        <v>1.187315660352547E-2</v>
-      </c>
-      <c r="H17" s="8">
+        <v>0.57450757758994209</v>
+      </c>
+      <c r="I17" s="7">
         <f t="shared" si="2"/>
-        <v>0.1187315660352547</v>
-      </c>
-      <c r="I17" s="8">
+        <v>1.1490151551798842</v>
+      </c>
+      <c r="J17" s="5">
+        <f>$B$31*F17*$B$10/($B$32*$B$22)</f>
+        <v>5144.769479274546</v>
+      </c>
+      <c r="K17" s="8">
         <f t="shared" si="3"/>
-        <v>0.2374631320705094</v>
-      </c>
-      <c r="J17" s="6">
+        <v>3.7311748601703269E-2</v>
+      </c>
+      <c r="L17" s="6">
+        <f>K17*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.6116791115498594</v>
+      </c>
+      <c r="M17" s="6">
         <f t="shared" si="4"/>
-        <v>27429.300809538741</v>
-      </c>
-      <c r="K17" s="9">
-        <f t="shared" si="5"/>
-        <v>2.4554630221472324E-2</v>
-      </c>
-      <c r="L17" s="7">
-        <f t="shared" si="6"/>
-        <v>1.168653125264788</v>
-      </c>
-      <c r="M17" s="7">
-        <f t="shared" si="7"/>
-        <v>0.08</v>
+        <v>0.38709677419354838</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B18">
-        <v>120</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="5">
-        <v>16</v>
-      </c>
-      <c r="F18" s="6">
+        <v>1.512041288</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="F18" s="5">
         <f t="shared" si="0"/>
-        <v>547.6288164542251</v>
-      </c>
-      <c r="G18" s="7">
+        <v>109.52576329084502</v>
+      </c>
+      <c r="G18" s="6">
+        <f>$B$11/(F18*$B$26)</f>
+        <v>5.5655421579025637E-2</v>
+      </c>
+      <c r="H18" s="7">
         <f t="shared" si="1"/>
-        <v>1.1131084315805126E-2</v>
-      </c>
-      <c r="H18" s="8">
+        <v>0.55655421579025632</v>
+      </c>
+      <c r="I18" s="7">
         <f t="shared" si="2"/>
-        <v>0.11131084315805126</v>
-      </c>
-      <c r="I18" s="8">
+        <v>1.1131084315805126</v>
+      </c>
+      <c r="J18" s="5">
+        <f>$B$31*F18*$B$10/($B$32*$B$22)</f>
+        <v>5310.729785057596</v>
+      </c>
+      <c r="K18" s="8">
         <f t="shared" si="3"/>
-        <v>0.22262168631610252</v>
-      </c>
-      <c r="J18" s="6">
+        <v>3.7016770932446055E-2</v>
+      </c>
+      <c r="L18" s="6">
+        <f>K18*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.5989375659045337</v>
+      </c>
+      <c r="M18" s="6">
         <f t="shared" si="4"/>
-        <v>29257.920863507992</v>
-      </c>
-      <c r="K18" s="9">
-        <f t="shared" si="5"/>
-        <v>2.4161629328799748E-2</v>
-      </c>
-      <c r="L18" s="7">
-        <f t="shared" si="6"/>
-        <v>1.1499486399065835</v>
-      </c>
-      <c r="M18" s="7">
-        <f t="shared" si="7"/>
-        <v>7.4999999999999997E-2</v>
+        <v>0.37499999999999994</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B19">
-        <v>1.512041288</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="5">
-        <v>17</v>
-      </c>
-      <c r="F19" s="6">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="E19" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="F19" s="5">
         <f t="shared" si="0"/>
-        <v>581.85561748261409</v>
-      </c>
-      <c r="G19" s="7">
+        <v>112.94844339368392</v>
+      </c>
+      <c r="G19" s="6">
+        <f>$B$11/(F19*$B$26)</f>
+        <v>5.3968893652388494E-2</v>
+      </c>
+      <c r="H19" s="7">
         <f t="shared" si="1"/>
-        <v>1.0476314650169533E-2</v>
-      </c>
-      <c r="H19" s="8">
+        <v>0.53968893652388494</v>
+      </c>
+      <c r="I19" s="7">
         <f t="shared" si="2"/>
-        <v>0.10476314650169533</v>
-      </c>
-      <c r="I19" s="8">
+        <v>1.0793778730477699</v>
+      </c>
+      <c r="J19" s="5">
+        <f>$B$31*F19*$B$10/($B$32*$B$22)</f>
+        <v>5476.690090840646</v>
+      </c>
+      <c r="K19" s="8">
         <f t="shared" si="3"/>
-        <v>0.20952629300339065</v>
-      </c>
-      <c r="J19" s="6">
+        <v>3.6733096612602163E-2</v>
+      </c>
+      <c r="L19" s="6">
+        <f>K19*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.5866842678708242</v>
+      </c>
+      <c r="M19" s="6">
         <f t="shared" si="4"/>
-        <v>31086.540917477243</v>
-      </c>
-      <c r="K19" s="9">
-        <f t="shared" si="5"/>
-        <v>2.3798193024256571E-2</v>
-      </c>
-      <c r="L19" s="7">
-        <f t="shared" si="6"/>
-        <v>1.1326512516214338</v>
-      </c>
-      <c r="M19" s="7">
-        <f t="shared" si="7"/>
-        <v>7.0588235294117646E-2</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="E20" s="5">
-        <v>18</v>
-      </c>
-      <c r="F20" s="6">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="F20" s="5">
         <f t="shared" si="0"/>
-        <v>616.0824185110032</v>
-      </c>
-      <c r="G20" s="7">
+        <v>116.37112349652283</v>
+      </c>
+      <c r="G20" s="6">
+        <f>$B$11/(F20*$B$26)</f>
+        <v>5.2381573250847663E-2</v>
+      </c>
+      <c r="H20" s="7">
         <f t="shared" si="1"/>
-        <v>9.8942971696045576E-3</v>
-      </c>
-      <c r="H20" s="8">
+        <v>0.52381573250847668</v>
+      </c>
+      <c r="I20" s="7">
         <f t="shared" si="2"/>
-        <v>9.8942971696045573E-2</v>
-      </c>
-      <c r="I20" s="8">
+        <v>1.0476314650169534</v>
+      </c>
+      <c r="J20" s="5">
+        <f>$B$31*F20*$B$10/($B$32*$B$22)</f>
+        <v>5642.6503966236951</v>
+      </c>
+      <c r="K20" s="8">
         <f t="shared" si="3"/>
-        <v>0.19788594339209115</v>
-      </c>
-      <c r="J20" s="6">
+        <v>3.6459969143513141E-2</v>
+      </c>
+      <c r="L20" s="6">
+        <f>K20*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.5748865405270789</v>
+      </c>
+      <c r="M20" s="6">
         <f t="shared" si="4"/>
-        <v>32915.160971446494</v>
-      </c>
-      <c r="K20" s="9">
-        <f t="shared" si="5"/>
-        <v>2.3460544460349245E-2</v>
-      </c>
-      <c r="L20" s="7">
-        <f t="shared" si="6"/>
-        <v>1.1165812051213486</v>
-      </c>
-      <c r="M20" s="7">
-        <f t="shared" si="7"/>
-        <v>6.6666666666666666E-2</v>
+        <v>0.35294117647058826</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>68.94</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="5">
-        <v>19</v>
-      </c>
-      <c r="F21" s="6">
+      <c r="E21" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="F21" s="5">
         <f t="shared" si="0"/>
-        <v>650.3092195393923</v>
-      </c>
-      <c r="G21" s="7">
+        <v>119.79380359936174</v>
+      </c>
+      <c r="G21" s="6">
+        <f>$B$11/(F21*$B$26)</f>
+        <v>5.0884956872252009E-2</v>
+      </c>
+      <c r="H21" s="7">
         <f t="shared" si="1"/>
-        <v>9.373544686993791E-3</v>
-      </c>
-      <c r="H21" s="8">
+        <v>0.50884956872252007</v>
+      </c>
+      <c r="I21" s="7">
         <f t="shared" si="2"/>
-        <v>9.37354468699379E-2</v>
-      </c>
-      <c r="I21" s="8">
+        <v>1.0176991374450401</v>
+      </c>
+      <c r="J21" s="5">
+        <f>$B$31*F21*$B$10/($B$32*$B$22)</f>
+        <v>5808.6107024067451</v>
+      </c>
+      <c r="K21" s="8">
         <f t="shared" si="3"/>
-        <v>0.1874708937398758</v>
-      </c>
-      <c r="J21" s="6">
+        <v>3.6196703050143823E-2</v>
+      </c>
+      <c r="L21" s="6">
+        <f>K21*$B$11*$B$31*$B$25*$B$20/(2*$B$10*$B$27)</f>
+        <v>1.5635147748134965</v>
+      </c>
+      <c r="M21" s="6">
         <f t="shared" si="4"/>
-        <v>34743.781025415738</v>
-      </c>
-      <c r="K21" s="9">
-        <f t="shared" si="5"/>
-        <v>2.3145566392478042E-2</v>
-      </c>
-      <c r="L21" s="7">
-        <f t="shared" si="6"/>
-        <v>1.1015901382599282</v>
-      </c>
-      <c r="M21" s="7">
-        <f t="shared" si="7"/>
-        <v>6.3157894736842107E-2</v>
+        <v>0.34285714285714286</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22">
-        <v>68.94</v>
-      </c>
-      <c r="C22" t="s">
+        <v>39.369999999999997</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23">
-        <v>39.369999999999997</v>
-      </c>
-      <c r="C23" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B24">
-        <v>60</v>
-      </c>
-      <c r="C24" s="16" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B25">
-        <v>1000</v>
-      </c>
-      <c r="C25" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B26">
-        <v>12</v>
-      </c>
-      <c r="C26" s="16" t="s">
+        <v>3.2810000000000001</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B27">
-        <v>3.2810000000000001</v>
-      </c>
-      <c r="C27" s="16" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28">
-        <v>1000</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>38</v>
-      </c>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="14"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="16"/>
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="15">
+        <f>(B13-32)*5/9</f>
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="17">
-        <f>(B13-32)*5/9</f>
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="B31" s="16">
+        <f>1000*B12/(B16*(B30+273.15))</f>
+        <v>1.1158695390957207</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="18">
-        <f>1000*B12/(B17*(B31+273.15))</f>
-        <v>1.2295117240090445</v>
+        <v>50</v>
+      </c>
+      <c r="B32" s="17">
+        <f>B18*(B30+273.15)^1.5/((B30+273.15+B17)*10^6)</f>
+        <v>1.8120567102806564E-5</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" s="19">
-        <f>B19*(B31+273.15)^1.5/((B31+273.15+B18)*10^6)</f>
-        <v>1.8120567102806564E-5</v>
+        <v>52</v>
+      </c>
+      <c r="B33" s="18">
+        <f>PI()*(B10/2)^2</f>
+        <v>7.5476763502494771E-4</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="20">
-        <f>PI()*(B10/2)^2</f>
-        <v>7.5476763502494771E-4</v>
+        <v>54</v>
+      </c>
+      <c r="B34" s="15">
+        <f>$B$12*$B$19</f>
+        <v>48.734400000000001</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="17">
-        <f>$B$12*$B$20</f>
-        <v>53.697600000000001</v>
+      <c r="A35" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="20">
+        <f>($B$12-$B$34)*$B$20</f>
+        <v>435.65599999999995</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="22">
-        <f>($B$12-$B$35)*$B$21</f>
-        <v>480.024</v>
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="20">
+        <f>-1*$B$3*$B$21-AVERAGE(L3:L21)</f>
+        <v>-642.83841799298114</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="22">
-        <f>-1*$B$3*$B$22-AVERAGE(L3:L21)</f>
-        <v>-483.97926740627173</v>
-      </c>
-      <c r="C37" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2627,8 +2646,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup scale="75" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>